<commit_message>
Preparar aplicación para despliegue en Streamlit Cloud
</commit_message>
<xml_diff>
--- a/EmpleosDIAN_2025.xlsx
+++ b/EmpleosDIAN_2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://diancolombia-my.sharepoint.com/personal/bhenaom_dian_gov_co/Documents/Escritorio/BRAYAN HENAO/2025/DOCUMENTOS PERSONALES/CONCURSO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Luis\Downloads\Empleos_dian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{97CE3CB5-8720-4714-948A-087C0DEDE099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BB0D06C-1582-4197-ADFD-CE9BCC391E49}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B64063-35C3-4044-A0F4-CA99F7DD7AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Empleos" sheetId="2" r:id="rId1"/>
@@ -4152,26 +4152,26 @@
   <dimension ref="A1:L325"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D98" sqref="A98:XFD98"/>
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="50.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.5703125" customWidth="1"/>
-    <col min="10" max="10" width="124.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="50.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.5546875" customWidth="1"/>
+    <col min="10" max="10" width="124.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="255.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4209,7 +4209,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>236565</v>
       </c>
@@ -4247,7 +4247,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>236566</v>
       </c>
@@ -4285,7 +4285,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>236567</v>
       </c>
@@ -4323,7 +4323,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>236568</v>
       </c>
@@ -4361,7 +4361,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>236569</v>
       </c>
@@ -4399,7 +4399,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>236570</v>
       </c>
@@ -4437,7 +4437,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>236571</v>
       </c>
@@ -4475,7 +4475,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>236573</v>
       </c>
@@ -4513,7 +4513,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>236574</v>
       </c>
@@ -4551,7 +4551,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>236575</v>
       </c>
@@ -4589,7 +4589,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>236576</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>236578</v>
       </c>
@@ -4665,7 +4665,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>236579</v>
       </c>
@@ -4703,7 +4703,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>236581</v>
       </c>
@@ -4741,7 +4741,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>236583</v>
       </c>
@@ -4779,7 +4779,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>236584</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>236586</v>
       </c>
@@ -4855,7 +4855,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>236587</v>
       </c>
@@ -4893,7 +4893,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>236589</v>
       </c>
@@ -4931,7 +4931,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>236590</v>
       </c>
@@ -4969,7 +4969,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>236591</v>
       </c>
@@ -5007,7 +5007,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>236592</v>
       </c>
@@ -5045,7 +5045,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>236594</v>
       </c>
@@ -5083,7 +5083,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>236596</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>236598</v>
       </c>
@@ -5159,7 +5159,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>236602</v>
       </c>
@@ -5197,7 +5197,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>236603</v>
       </c>
@@ -5235,7 +5235,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>236605</v>
       </c>
@@ -5273,7 +5273,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>236608</v>
       </c>
@@ -5311,7 +5311,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>236610</v>
       </c>
@@ -5349,7 +5349,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>236611</v>
       </c>
@@ -5387,7 +5387,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>236614</v>
       </c>
@@ -5425,7 +5425,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>236617</v>
       </c>
@@ -5463,7 +5463,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>236619</v>
       </c>
@@ -5501,7 +5501,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>236621</v>
       </c>
@@ -5539,7 +5539,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>236622</v>
       </c>
@@ -5577,7 +5577,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>236626</v>
       </c>
@@ -5615,7 +5615,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>236628</v>
       </c>
@@ -5653,7 +5653,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>236631</v>
       </c>
@@ -5691,7 +5691,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>236633</v>
       </c>
@@ -5729,7 +5729,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>236634</v>
       </c>
@@ -5767,7 +5767,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>236635</v>
       </c>
@@ -5805,7 +5805,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>236636</v>
       </c>
@@ -5843,7 +5843,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>236637</v>
       </c>
@@ -5881,7 +5881,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>236638</v>
       </c>
@@ -5919,7 +5919,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>236639</v>
       </c>
@@ -5957,7 +5957,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>236640</v>
       </c>
@@ -5995,7 +5995,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>236641</v>
       </c>
@@ -6033,7 +6033,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>236642</v>
       </c>
@@ -6071,7 +6071,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>236643</v>
       </c>
@@ -6109,7 +6109,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>236644</v>
       </c>
@@ -6147,7 +6147,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>236646</v>
       </c>
@@ -6185,7 +6185,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>236648</v>
       </c>
@@ -6223,7 +6223,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>236650</v>
       </c>
@@ -6261,7 +6261,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>236651</v>
       </c>
@@ -6299,7 +6299,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>236653</v>
       </c>
@@ -6337,7 +6337,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>236654</v>
       </c>
@@ -6375,7 +6375,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>236656</v>
       </c>
@@ -6413,7 +6413,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>236657</v>
       </c>
@@ -6451,7 +6451,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>236659</v>
       </c>
@@ -6489,7 +6489,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>236660</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>236664</v>
       </c>
@@ -6565,7 +6565,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>236665</v>
       </c>
@@ -6603,7 +6603,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>236667</v>
       </c>
@@ -6641,7 +6641,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>236668</v>
       </c>
@@ -6679,7 +6679,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>236669</v>
       </c>
@@ -6717,7 +6717,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>236670</v>
       </c>
@@ -6755,7 +6755,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>236671</v>
       </c>
@@ -6793,7 +6793,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>236672</v>
       </c>
@@ -6831,7 +6831,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>236673</v>
       </c>
@@ -6869,7 +6869,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>236674</v>
       </c>
@@ -6907,7 +6907,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>236675</v>
       </c>
@@ -6945,7 +6945,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>236676</v>
       </c>
@@ -6983,7 +6983,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>236677</v>
       </c>
@@ -7021,7 +7021,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>236679</v>
       </c>
@@ -7059,7 +7059,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>236680</v>
       </c>
@@ -7097,7 +7097,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>236681</v>
       </c>
@@ -7135,7 +7135,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>236682</v>
       </c>
@@ -7173,7 +7173,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>236683</v>
       </c>
@@ -7211,7 +7211,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>236684</v>
       </c>
@@ -7249,7 +7249,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>236685</v>
       </c>
@@ -7287,7 +7287,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>236687</v>
       </c>
@@ -7325,7 +7325,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>236688</v>
       </c>
@@ -7363,7 +7363,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>236689</v>
       </c>
@@ -7401,7 +7401,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>236690</v>
       </c>
@@ -7439,7 +7439,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>236692</v>
       </c>
@@ -7477,7 +7477,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>236693</v>
       </c>
@@ -7515,7 +7515,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>236694</v>
       </c>
@@ -7553,7 +7553,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="90" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>236695</v>
       </c>
@@ -7591,7 +7591,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>236696</v>
       </c>
@@ -7629,7 +7629,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="92" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>236699</v>
       </c>
@@ -7667,7 +7667,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>236700</v>
       </c>
@@ -7705,7 +7705,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>236701</v>
       </c>
@@ -7743,7 +7743,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>236702</v>
       </c>
@@ -7781,7 +7781,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>236703</v>
       </c>
@@ -7819,7 +7819,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="97" spans="1:12" ht="0.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" ht="0.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>236704</v>
       </c>
@@ -7857,7 +7857,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>236705</v>
       </c>
@@ -7895,7 +7895,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>236706</v>
       </c>
@@ -7933,7 +7933,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>236707</v>
       </c>
@@ -7971,7 +7971,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>236708</v>
       </c>
@@ -8009,7 +8009,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>236709</v>
       </c>
@@ -8047,7 +8047,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>236710</v>
       </c>
@@ -8085,7 +8085,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>236711</v>
       </c>
@@ -8123,7 +8123,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>236712</v>
       </c>
@@ -8161,7 +8161,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>236713</v>
       </c>
@@ -8199,7 +8199,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>236714</v>
       </c>
@@ -8237,7 +8237,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>236715</v>
       </c>
@@ -8275,7 +8275,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>236718</v>
       </c>
@@ -8313,7 +8313,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>236721</v>
       </c>
@@ -8351,7 +8351,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>236722</v>
       </c>
@@ -8389,7 +8389,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="112" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>236724</v>
       </c>
@@ -8427,7 +8427,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>236726</v>
       </c>
@@ -8465,7 +8465,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>236727</v>
       </c>
@@ -8503,7 +8503,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>236731</v>
       </c>
@@ -8541,7 +8541,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>236732</v>
       </c>
@@ -8579,7 +8579,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>236733</v>
       </c>
@@ -8617,7 +8617,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>236734</v>
       </c>
@@ -8655,7 +8655,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>236735</v>
       </c>
@@ -8693,7 +8693,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>236738</v>
       </c>
@@ -8731,7 +8731,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>236739</v>
       </c>
@@ -8769,7 +8769,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>236740</v>
       </c>
@@ -8807,7 +8807,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>236741</v>
       </c>
@@ -8845,7 +8845,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>236742</v>
       </c>
@@ -8883,7 +8883,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>236744</v>
       </c>
@@ -8921,7 +8921,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>236745</v>
       </c>
@@ -8959,7 +8959,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>236747</v>
       </c>
@@ -8997,7 +8997,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>236756</v>
       </c>
@@ -9035,7 +9035,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>236760</v>
       </c>
@@ -9073,7 +9073,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>236761</v>
       </c>
@@ -9111,7 +9111,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>236762</v>
       </c>
@@ -9149,7 +9149,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>236764</v>
       </c>
@@ -9187,7 +9187,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>236765</v>
       </c>
@@ -9225,7 +9225,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>236767</v>
       </c>
@@ -9263,7 +9263,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>236769</v>
       </c>
@@ -9301,7 +9301,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>236771</v>
       </c>
@@ -9339,7 +9339,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>236772</v>
       </c>
@@ -9377,7 +9377,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>236776</v>
       </c>
@@ -9415,7 +9415,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="139" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>236778</v>
       </c>
@@ -9453,7 +9453,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>236779</v>
       </c>
@@ -9491,7 +9491,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="141" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>236780</v>
       </c>
@@ -9529,7 +9529,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>236781</v>
       </c>
@@ -9567,7 +9567,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>236782</v>
       </c>
@@ -9605,7 +9605,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>236785</v>
       </c>
@@ -9643,7 +9643,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>236787</v>
       </c>
@@ -9681,7 +9681,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="146" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>236791</v>
       </c>
@@ -9719,7 +9719,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="147" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>236792</v>
       </c>
@@ -9757,7 +9757,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>236793</v>
       </c>
@@ -9795,7 +9795,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>236794</v>
       </c>
@@ -9833,7 +9833,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="150" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>236795</v>
       </c>
@@ -9871,7 +9871,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="151" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>236796</v>
       </c>
@@ -9909,7 +9909,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="152" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>236798</v>
       </c>
@@ -9947,7 +9947,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="153" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>236799</v>
       </c>
@@ -9985,7 +9985,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>236800</v>
       </c>
@@ -10023,7 +10023,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>236801</v>
       </c>
@@ -10061,7 +10061,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>236802</v>
       </c>
@@ -10099,7 +10099,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>236804</v>
       </c>
@@ -10137,7 +10137,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>236805</v>
       </c>
@@ -10175,7 +10175,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>236806</v>
       </c>
@@ -10213,7 +10213,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="160" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>236807</v>
       </c>
@@ -10251,7 +10251,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="161" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>236808</v>
       </c>
@@ -10289,7 +10289,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="162" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>236809</v>
       </c>
@@ -10327,7 +10327,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="163" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>236810</v>
       </c>
@@ -10365,7 +10365,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="164" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>236819</v>
       </c>
@@ -10403,7 +10403,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="165" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>236825</v>
       </c>
@@ -10441,7 +10441,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="166" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>236826</v>
       </c>
@@ -10479,7 +10479,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="167" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>236828</v>
       </c>
@@ -10517,7 +10517,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="168" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>236831</v>
       </c>
@@ -10555,7 +10555,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="169" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>236840</v>
       </c>
@@ -10593,7 +10593,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="170" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>236842</v>
       </c>
@@ -10631,7 +10631,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="171" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>236844</v>
       </c>
@@ -10669,7 +10669,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="172" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>236845</v>
       </c>
@@ -10707,7 +10707,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="173" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>236847</v>
       </c>
@@ -10745,7 +10745,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="174" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>236849</v>
       </c>
@@ -10783,7 +10783,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="175" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>236851</v>
       </c>
@@ -10821,7 +10821,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="176" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>236852</v>
       </c>
@@ -10859,7 +10859,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="177" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>236853</v>
       </c>
@@ -10897,7 +10897,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="178" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>236854</v>
       </c>
@@ -10935,7 +10935,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="179" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>236855</v>
       </c>
@@ -10973,7 +10973,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="180" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>236857</v>
       </c>
@@ -11011,7 +11011,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="181" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>236859</v>
       </c>
@@ -11049,7 +11049,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="182" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>236860</v>
       </c>
@@ -11087,7 +11087,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="183" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>236861</v>
       </c>
@@ -11125,7 +11125,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="184" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>236863</v>
       </c>
@@ -11163,7 +11163,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="185" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>236865</v>
       </c>
@@ -11201,7 +11201,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="186" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>236866</v>
       </c>
@@ -11239,7 +11239,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="187" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>236867</v>
       </c>
@@ -11277,7 +11277,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="188" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>236868</v>
       </c>
@@ -11315,7 +11315,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="189" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>236869</v>
       </c>
@@ -11353,7 +11353,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="190" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>236870</v>
       </c>
@@ -11391,7 +11391,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="191" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>236871</v>
       </c>
@@ -11429,7 +11429,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="192" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>236872</v>
       </c>
@@ -11467,7 +11467,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="193" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>236874</v>
       </c>
@@ -11505,7 +11505,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="194" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>236875</v>
       </c>
@@ -11543,7 +11543,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="195" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>236877</v>
       </c>
@@ -11581,7 +11581,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="196" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>236879</v>
       </c>
@@ -11619,7 +11619,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="197" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>236881</v>
       </c>
@@ -11657,7 +11657,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="198" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>236882</v>
       </c>
@@ -11695,7 +11695,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="199" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>236883</v>
       </c>
@@ -11733,7 +11733,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="200" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>236885</v>
       </c>
@@ -11771,7 +11771,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="201" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>236887</v>
       </c>
@@ -11809,7 +11809,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="202" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>236888</v>
       </c>
@@ -11847,7 +11847,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="203" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>236889</v>
       </c>
@@ -11885,7 +11885,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="204" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>236891</v>
       </c>
@@ -11923,7 +11923,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="205" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>236892</v>
       </c>
@@ -11961,7 +11961,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="206" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>236893</v>
       </c>
@@ -11999,7 +11999,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="207" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>236894</v>
       </c>
@@ -12037,7 +12037,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="208" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>236895</v>
       </c>
@@ -12075,7 +12075,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="209" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>236897</v>
       </c>
@@ -12113,7 +12113,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>236899</v>
       </c>
@@ -12151,7 +12151,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="211" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>236900</v>
       </c>
@@ -12189,7 +12189,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="212" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>236901</v>
       </c>
@@ -12227,7 +12227,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="213" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>236902</v>
       </c>
@@ -12265,7 +12265,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="214" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>236904</v>
       </c>
@@ -12303,7 +12303,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="215" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>236906</v>
       </c>
@@ -12341,7 +12341,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="216" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>236908</v>
       </c>
@@ -12379,7 +12379,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="217" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>236909</v>
       </c>
@@ -12417,7 +12417,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="218" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>236911</v>
       </c>
@@ -12455,7 +12455,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="219" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>236916</v>
       </c>
@@ -12493,7 +12493,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="220" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>242398</v>
       </c>
@@ -12531,7 +12531,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="221" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>242574</v>
       </c>
@@ -12569,7 +12569,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="222" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>242576</v>
       </c>
@@ -12607,7 +12607,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="223" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>242577</v>
       </c>
@@ -12645,7 +12645,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="224" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>242578</v>
       </c>
@@ -12683,7 +12683,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="225" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>242579</v>
       </c>
@@ -12721,7 +12721,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="226" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>242580</v>
       </c>
@@ -12759,7 +12759,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="227" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>242581</v>
       </c>
@@ -12797,7 +12797,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="228" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>242582</v>
       </c>
@@ -12835,7 +12835,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="229" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>242583</v>
       </c>
@@ -12873,7 +12873,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="230" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>242584</v>
       </c>
@@ -12911,7 +12911,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="231" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>242585</v>
       </c>
@@ -12949,7 +12949,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="232" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>242586</v>
       </c>
@@ -12987,7 +12987,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="233" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>242587</v>
       </c>
@@ -13025,7 +13025,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="234" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>242588</v>
       </c>
@@ -13063,7 +13063,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="235" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>242589</v>
       </c>
@@ -13101,7 +13101,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="236" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>242590</v>
       </c>
@@ -13139,7 +13139,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="237" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>242591</v>
       </c>
@@ -13177,7 +13177,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="238" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>242604</v>
       </c>
@@ -13215,7 +13215,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="239" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>242605</v>
       </c>
@@ -13253,7 +13253,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="240" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>242606</v>
       </c>
@@ -13291,7 +13291,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="241" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>242607</v>
       </c>
@@ -13329,7 +13329,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="242" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>242608</v>
       </c>
@@ -13367,7 +13367,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="243" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>242609</v>
       </c>
@@ -13405,7 +13405,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="244" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>242610</v>
       </c>
@@ -13443,7 +13443,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="245" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>242612</v>
       </c>
@@ -13481,7 +13481,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="246" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>242613</v>
       </c>
@@ -13519,7 +13519,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="247" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>242614</v>
       </c>
@@ -13557,7 +13557,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="248" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>242615</v>
       </c>
@@ -13595,7 +13595,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="249" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>242616</v>
       </c>
@@ -13633,7 +13633,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="250" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>242617</v>
       </c>
@@ -13671,7 +13671,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="251" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>242618</v>
       </c>
@@ -13709,7 +13709,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="252" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>242619</v>
       </c>
@@ -13747,7 +13747,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="253" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>242620</v>
       </c>
@@ -13785,7 +13785,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="254" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>242621</v>
       </c>
@@ -13823,7 +13823,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="255" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>242622</v>
       </c>
@@ -13861,7 +13861,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="256" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>242623</v>
       </c>
@@ -13899,7 +13899,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="257" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>242624</v>
       </c>
@@ -13937,7 +13937,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="258" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>242625</v>
       </c>
@@ -13975,7 +13975,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="259" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>242627</v>
       </c>
@@ -14013,7 +14013,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="260" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>242628</v>
       </c>
@@ -14051,7 +14051,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="261" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>242629</v>
       </c>
@@ -14089,7 +14089,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="262" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>242630</v>
       </c>
@@ -14127,7 +14127,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="263" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>242631</v>
       </c>
@@ -14165,7 +14165,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="264" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>242632</v>
       </c>
@@ -14203,7 +14203,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="265" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>242633</v>
       </c>
@@ -14241,7 +14241,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="266" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>242634</v>
       </c>
@@ -14279,7 +14279,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="267" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>242635</v>
       </c>
@@ -14317,7 +14317,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="268" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>242636</v>
       </c>
@@ -14355,7 +14355,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="269" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>242637</v>
       </c>
@@ -14393,7 +14393,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="270" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>242638</v>
       </c>
@@ -14431,7 +14431,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="271" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>242639</v>
       </c>
@@ -14469,7 +14469,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="272" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>242640</v>
       </c>
@@ -14507,7 +14507,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="273" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>242641</v>
       </c>
@@ -14545,7 +14545,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="274" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>242642</v>
       </c>
@@ -14583,7 +14583,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="275" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>242643</v>
       </c>
@@ -14621,7 +14621,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="276" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>242644</v>
       </c>
@@ -14659,7 +14659,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="277" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>242645</v>
       </c>
@@ -14697,7 +14697,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="278" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>242646</v>
       </c>
@@ -14735,7 +14735,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="279" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>242647</v>
       </c>
@@ -14773,7 +14773,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="280" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>242648</v>
       </c>
@@ -14811,7 +14811,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="281" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>242649</v>
       </c>
@@ -14849,7 +14849,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="282" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>242650</v>
       </c>
@@ -14887,7 +14887,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="283" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>242651</v>
       </c>
@@ -14925,7 +14925,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="284" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>242652</v>
       </c>
@@ -14963,7 +14963,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="285" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>242653</v>
       </c>
@@ -15001,7 +15001,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="286" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>242654</v>
       </c>
@@ -15039,7 +15039,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="287" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>242655</v>
       </c>
@@ -15077,7 +15077,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="288" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>242656</v>
       </c>
@@ -15115,7 +15115,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="289" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>242657</v>
       </c>
@@ -15153,7 +15153,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="290" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>242658</v>
       </c>
@@ -15191,7 +15191,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="291" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>242659</v>
       </c>
@@ -15229,7 +15229,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="292" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>242660</v>
       </c>
@@ -15267,7 +15267,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="293" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>242661</v>
       </c>
@@ -15305,7 +15305,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="294" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>242662</v>
       </c>
@@ -15343,7 +15343,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="295" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>242663</v>
       </c>
@@ -15381,7 +15381,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="296" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>242664</v>
       </c>
@@ -15419,7 +15419,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="297" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>242665</v>
       </c>
@@ -15457,7 +15457,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="298" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>242666</v>
       </c>
@@ -15495,7 +15495,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="299" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>242667</v>
       </c>
@@ -15533,7 +15533,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="300" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>242669</v>
       </c>
@@ -15571,7 +15571,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="301" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>242670</v>
       </c>
@@ -15609,7 +15609,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="302" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>242671</v>
       </c>
@@ -15647,7 +15647,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="303" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>242672</v>
       </c>
@@ -15685,7 +15685,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="304" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>242679</v>
       </c>
@@ -15723,7 +15723,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="305" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A305">
         <v>242680</v>
       </c>
@@ -15761,7 +15761,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="306" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>242681</v>
       </c>
@@ -15799,7 +15799,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="307" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>242682</v>
       </c>
@@ -15837,7 +15837,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="308" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A308">
         <v>242683</v>
       </c>
@@ -15875,7 +15875,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="309" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>242684</v>
       </c>
@@ -15913,7 +15913,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="310" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>242686</v>
       </c>
@@ -15951,7 +15951,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="311" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>242687</v>
       </c>
@@ -15989,7 +15989,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="312" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>242690</v>
       </c>
@@ -16027,7 +16027,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="313" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>242691</v>
       </c>
@@ -16065,7 +16065,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="314" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A314">
         <v>242692</v>
       </c>
@@ -16103,7 +16103,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="315" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A315">
         <v>242693</v>
       </c>
@@ -16141,7 +16141,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="316" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A316">
         <v>242694</v>
       </c>
@@ -16179,7 +16179,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="317" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A317">
         <v>242695</v>
       </c>
@@ -16217,7 +16217,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="318" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A318">
         <v>242696</v>
       </c>
@@ -16255,7 +16255,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="319" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A319">
         <v>242697</v>
       </c>
@@ -16293,7 +16293,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="320" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A320">
         <v>242698</v>
       </c>
@@ -16331,7 +16331,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="321" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A321">
         <v>242699</v>
       </c>
@@ -16369,7 +16369,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="322" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A322">
         <v>242701</v>
       </c>
@@ -16407,7 +16407,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="323" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A323">
         <v>242702</v>
       </c>
@@ -16445,7 +16445,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="324" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A324">
         <v>242703</v>
       </c>
@@ -16483,7 +16483,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="325" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A325">
         <v>244171</v>
       </c>

</xml_diff>